<commit_message>
Commit Changes feb 25 2020
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D4C282A0-6EA7-460E-8296-F0563D1627E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sulta\git\Framework\Framework\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2EAD1F-0095-4DBE-9211-39909FA97363}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15435" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -347,7 +351,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>